<commit_message>
tracability link matrix updated
</commit_message>
<xml_diff>
--- a/6- Traceability link matrix/Traceability Link Matrix.xlsx
+++ b/6- Traceability link matrix/Traceability Link Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\CS414 Group Project\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakot\IdeaProjects\cs414-f20-public_class_TeamD\6- Traceability link matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC08EABC-D544-4BBD-95A9-2384F3F7E088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A30AE8E-CFDD-4E26-84CD-62293CFFE32E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51405" yWindow="2565" windowWidth="11655" windowHeight="11385" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="599" xr2:uid="{6F3B0F6D-D4FA-43ED-9BE5-68FBBAC2F32D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="67">
   <si>
     <t>User Stories</t>
   </si>
@@ -190,6 +189,51 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>BoardGame</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>InviteBox</t>
+  </si>
+  <si>
+    <t>MatchHistory</t>
+  </si>
+  <si>
+    <t>Ping</t>
+  </si>
+  <si>
+    <t>Searching</t>
+  </si>
+  <si>
+    <t>GameplayController</t>
+  </si>
+  <si>
+    <t>Helper</t>
+  </si>
+  <si>
+    <t>AcceptInvite</t>
+  </si>
+  <si>
+    <t>GetInvites</t>
+  </si>
+  <si>
+    <t>InvitesController</t>
+  </si>
+  <si>
+    <t>SendInvite</t>
+  </si>
+  <si>
+    <t>LobbyController</t>
+  </si>
+  <si>
+    <t>MatchHistoryController</t>
+  </si>
+  <si>
+    <t>RetrievePlayers</t>
   </si>
 </sst>
 </file>
@@ -245,13 +289,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,226 +617,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C21C376-BCAA-4BB5-9BB8-5CF377B37712}">
-  <dimension ref="A1:AM17"/>
+  <dimension ref="A1:BL17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL8" sqref="AL8"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BE10" sqref="BE10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.1015625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.47265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.20703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="4.89453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.62890625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.05078125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.05078125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.89453125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.1015625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.15625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.15625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.9453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.89453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.62890625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.3125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.62890625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.89453125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.734375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.20703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="6.26171875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.89453125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.47265625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.47265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="4.89453125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="19.47265625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.1015625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.15625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.1015625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.15625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.41796875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="5.578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.20703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="D1" s="1"/>
+      <c r="S1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="P2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" t="s">
+      <c r="Q2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="V2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Y2" t="s">
         <v>9</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Z2" t="s">
         <v>32</v>
       </c>
-      <c r="T2" t="s">
+      <c r="AA2" t="s">
         <v>20</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AB2" t="s">
         <v>33</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AC2" t="s">
         <v>2</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AD2" t="s">
         <v>47</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AE2" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AF2" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AG2" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AH2" t="s">
         <v>36</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>33</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH2" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="BI2" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="BJ2" t="s">
         <v>45</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL2" t="s">
+      <c r="BK2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BL2" t="s">
         <v>49</v>
       </c>
-      <c r="AM2" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
-      <c r="V3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="X3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
+      <c r="AC3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
@@ -793,17 +942,30 @@
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
-      <c r="AL3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AL3" s="3"/>
       <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AP3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS3" s="3"/>
+      <c r="BF3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -839,49 +1001,55 @@
       <c r="AK4" s="3"/>
       <c r="AL4" s="3"/>
       <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
+      <c r="AA5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
@@ -891,19 +1059,30 @@
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
-      <c r="AL5" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AL5" s="3"/>
       <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS5" s="3"/>
+      <c r="BD5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
         <v>51</v>
       </c>
@@ -911,33 +1090,41 @@
         <v>51</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="M6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
+      <c r="S6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
@@ -951,19 +1138,42 @@
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
-      <c r="AL6" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS6" s="3"/>
+      <c r="AT6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
         <v>51</v>
       </c>
@@ -971,30 +1181,38 @@
         <v>51</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="M7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
+      <c r="S7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -1009,20 +1227,47 @@
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
-      <c r="AL7" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS7" s="3"/>
+      <c r="AT7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -1055,16 +1300,22 @@
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
       <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AS8" s="3"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -1097,47 +1348,57 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="3"/>
       <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+      <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
+      <c r="AS9" s="3"/>
+      <c r="BB9" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="K10" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
+      <c r="X10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
@@ -1149,17 +1410,48 @@
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
-      <c r="AL10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AL10" s="3"/>
       <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="3"/>
+      <c r="AR10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS10" s="3"/>
+      <c r="AZ10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1177,24 +1469,20 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
+      <c r="V11" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="W11" s="3"/>
-      <c r="X11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
+      <c r="AE11" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="AF11" s="3" t="s">
         <v>51</v>
       </c>
@@ -1210,37 +1498,52 @@
       <c r="AJ11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AK11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL11" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
       <c r="AM11" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="AN11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="M12" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
@@ -1262,18 +1565,24 @@
       <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
+      <c r="AI12" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
       <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="3"/>
+      <c r="AP12" s="3"/>
+      <c r="AQ12" s="3"/>
+      <c r="AR12" s="3"/>
+      <c r="AS12" s="3"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1309,13 +1618,17 @@
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
       <c r="AM13" s="3"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="3"/>
+      <c r="AP13" s="3"/>
+      <c r="AQ13" s="3"/>
+      <c r="AR13" s="3"/>
+      <c r="AS13" s="3"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1346,18 +1659,32 @@
       <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
-      <c r="AJ14" s="3"/>
+      <c r="AI14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="AK14" s="3"/>
       <c r="AL14" s="3"/>
       <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1377,23 +1704,13 @@
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
-      <c r="X15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA15" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
-      <c r="AD15" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="AD15" s="3"/>
       <c r="AE15" s="3" t="s">
         <v>51</v>
       </c>
@@ -1421,13 +1738,32 @@
       <c r="AM15" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="AN15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1463,13 +1799,23 @@
       <c r="AK16" s="3"/>
       <c r="AL16" s="3"/>
       <c r="AM16" s="3"/>
+      <c r="AN16" s="3"/>
+      <c r="AO16" s="3"/>
+      <c r="AP16" s="3"/>
+      <c r="AQ16" s="3"/>
+      <c r="AR16" s="3"/>
+      <c r="AS16" s="3"/>
     </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:45" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1500,11 +1846,19 @@
       <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
+      <c r="AI17" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
       <c r="AL17" s="3"/>
       <c r="AM17" s="3"/>
+      <c r="AN17" s="3"/>
+      <c r="AO17" s="3"/>
+      <c r="AP17" s="3"/>
+      <c r="AQ17" s="3"/>
+      <c r="AR17" s="3"/>
+      <c r="AS17" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>